<commit_message>
update French translation (automatic)
</commit_message>
<xml_diff>
--- a/nomenclature.xlsx
+++ b/nomenclature.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">English</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Polish</t>
   </si>
   <si>
+    <t xml:space="preserve">French</t>
+  </si>
+  <si>
     <t xml:space="preserve">tag</t>
   </si>
   <si>
@@ -52,16 +55,46 @@
     <t xml:space="preserve">(etiketa/etikety)</t>
   </si>
   <si>
+    <t xml:space="preserve">(étiquette)</t>
+  </si>
+  <si>
     <t xml:space="preserve">template</t>
   </si>
   <si>
     <t xml:space="preserve">Vorlage</t>
   </si>
   <si>
+    <t xml:space="preserve">(mod`ele)</t>
+  </si>
+  <si>
     <t xml:space="preserve">area</t>
   </si>
   <si>
     <t xml:space="preserve">plocha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freehand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pismo odręczne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(écriture)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterprise</t>
   </si>
 </sst>
 </file>
@@ -242,10 +275,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.640625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,35 +305,76 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Greek translation (automatic)
</commit_message>
<xml_diff>
--- a/nomenclature.xlsx
+++ b/nomenclature.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">English</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">French</t>
   </si>
   <si>
+    <t xml:space="preserve">Greek</t>
+  </si>
+  <si>
     <t xml:space="preserve">tag</t>
   </si>
   <si>
@@ -55,7 +58,10 @@
     <t xml:space="preserve">(etiketa/etikety)</t>
   </si>
   <si>
-    <t xml:space="preserve">(étiquette)</t>
+    <t xml:space="preserve">(étiquette) [alternative: balise]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ετικέτες)</t>
   </si>
   <si>
     <t xml:space="preserve">template</t>
@@ -92,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Business</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise</t>
   </si>
 </sst>
 </file>
@@ -275,15 +278,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.640625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="23.61"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,73 +313,76 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my corrections for Dutch
</commit_message>
<xml_diff>
--- a/nomenclature.xlsx
+++ b/nomenclature.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t xml:space="preserve">English</t>
   </si>
@@ -46,6 +46,12 @@
     <t xml:space="preserve">Greek</t>
   </si>
   <si>
+    <t xml:space="preserve">Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
     <t xml:space="preserve">tag</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">(ετικέτες)</t>
   </si>
   <si>
+    <t xml:space="preserve">etiket</t>
+  </si>
+  <si>
     <t xml:space="preserve">template</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t xml:space="preserve">(mod`ele)</t>
   </si>
   <si>
+    <t xml:space="preserve">Sjabloon</t>
+  </si>
+  <si>
     <t xml:space="preserve">area</t>
   </si>
   <si>
@@ -98,6 +110,132 @@
   </si>
   <si>
     <t xml:space="preserve">Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">licentie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(element)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mijl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">are </t>
+  </si>
+  <si>
+    <t xml:space="preserve">are</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hectare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radialen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gradians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imperial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US paper size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(letter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(legal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lijnkap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the editing tool name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zähler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teller / teltool ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tekenblad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptobject type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabel / tafel ?</t>
   </si>
 </sst>
 </file>
@@ -112,6 +250,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -132,12 +271,14 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -188,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +339,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,15 +423,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.640625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="23.61"/>
   </cols>
@@ -316,35 +463,38 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -352,37 +502,237 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>